<commit_message>
change to the schema and cell_list to make compatible with the importers
</commit_message>
<xml_diff>
--- a/tests/test_data/01_raw/abuse/cell_list.xlsx
+++ b/tests/test_data/01_raw/abuse/cell_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdeange\PycharmProjects\battery-archive-sandbox\data\data_set_samples\abuse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdeange\PycharmProjects\battery-archive-sandbox-2\tests\test_data\01_raw\abuse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138E6542-C88A-40C9-A5E6-9CF3B4FB9A9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C64622-9CCD-4D9C-9591-22C75D778E72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{07EF3D65-9BA3-43DB-B014-0F8C59FBB292}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>NMC</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>sample_1</t>
+  </si>
+  <si>
+    <t>mapping</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -183,12 +189,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,7 +514,7 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,6 +579,9 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="X1" s="4"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -619,6 +630,9 @@
       <c r="O2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="P2" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -665,6 +679,9 @@
       </c>
       <c r="O3" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>